<commit_message>
Adjust Excel download/upload to include folders and parents
</commit_message>
<xml_diff>
--- a/public/Simulationsvorlage.xlsx
+++ b/public/Simulationsvorlage.xlsx
@@ -3,19 +3,26 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28227"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AF010CE7-CED0-4307-BE43-F111A3BA7238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0030B4C-7661-4B76-A189-062F1B1A69F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Seiten" sheetId="2" r:id="rId1"/>
+    <sheet name="Ordner" sheetId="1" r:id="rId1"/>
+    <sheet name="Seiten" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>In Ordner</t>
+  </si>
   <si>
     <t>Titel</t>
   </si>
@@ -23,16 +30,34 @@
     <t>Beschreibung</t>
   </si>
   <si>
-    <t>Ihre erste Seite</t>
-  </si>
-  <si>
-    <t>Eine andere Seite</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Die Seitenbeschreibung ist mit &lt;strong&gt;HTML&lt;/strong&gt; formatiert.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>Sie können ihn auch als reinen Text eingeben.</t>
+    <t>Titel eines Seitenordners</t>
+  </si>
+  <si>
+    <t>Ein weiterer Ordner</t>
+  </si>
+  <si>
+    <t>Beispieltitel</t>
+  </si>
+  <si>
+    <t>Zweite Seite</t>
+  </si>
+  <si>
+    <t>Dritte Seite</t>
+  </si>
+  <si>
+    <t>Titel der letzten Seite</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Die Beschreibung ist normalerweise als &lt;strong&gt;HTML&lt;/strong&gt; formatiert.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Die Beschreibung ist das, was auf der Seite angezeigt wird.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Es ist auch möglich, normalen Text zu verwenden. Wir werden das Beste daraus machen.</t>
+  </si>
+  <si>
+    <t>Dies ist der Inhalt, der auf der letzten Seite angezeigt wird.</t>
   </si>
 </sst>
 </file>
@@ -414,41 +439,119 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28" customWidth="1"/>
-    <col min="2" max="2" width="80" customWidth="1"/>
+    <col min="1" max="1" width="23" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" customWidth="1"/>
+    <col min="3" max="3" width="19.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.33203125" customWidth="1"/>
+    <col min="2" max="2" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.21875" customWidth="1"/>
+    <col min="4" max="4" width="80" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update simulation Excel template
</commit_message>
<xml_diff>
--- a/public/Simulationsvorlage.xlsx
+++ b/public/Simulationsvorlage.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28324"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0030B4C-7661-4B76-A189-062F1B1A69F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B4D8BAD-A9B2-41CE-8EE0-C8F963EEB59E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ordner" sheetId="1" r:id="rId1"/>
@@ -54,10 +54,11 @@
     <t>&lt;p&gt;Die Beschreibung ist das, was auf der Seite angezeigt wird.&lt;/p&gt;</t>
   </si>
   <si>
-    <t>Es ist auch möglich, normalen Text zu verwenden. Wir werden das Beste daraus machen.</t>
-  </si>
-  <si>
     <t>Dies ist der Inhalt, der auf der letzten Seite angezeigt wird.</t>
+  </si>
+  <si>
+    <t>Es ist auch möglich, normalen Text zu verwenden. Wir werden das Beste daraus machen.
+Verwenden Sie die Tastenkombination alt+enter in Excel, um Zeilenumbrüche hinzuzufügen.</t>
   </si>
 </sst>
 </file>
@@ -98,9 +99,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,14 +447,14 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" customWidth="1"/>
-    <col min="3" max="3" width="19.5546875" customWidth="1"/>
+    <col min="1" max="1" width="2.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -485,15 +489,15 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.33203125" customWidth="1"/>
-    <col min="2" max="2" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.21875" customWidth="1"/>
-    <col min="4" max="4" width="80" customWidth="1"/>
+    <col min="1" max="1" width="2.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="76.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -512,7 +516,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -523,7 +527,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -532,26 +536,26 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" t="s">
-        <v>12</v>
+      <c r="D4" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>